<commit_message>
servicios, contacto mail, footer, nav
</commit_message>
<xml_diff>
--- a/netlify/functions/Servicios.xlsx
+++ b/netlify/functions/Servicios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio Aguilera\Desktop\Trabajo (SPA)\AutogesCL\netlify\functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio Aguilera\Desktop\Trabajo (SPA)\MasAutomatizacion\netlify\functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E945C525-E867-4632-A480-3E7C9EC8D9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F8796D-5BBB-4CED-AB6C-DD41238AD036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+  <si>
+    <t>IdServicio</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
   <si>
     <t>Service Title</t>
   </si>
@@ -52,7 +58,28 @@
     <t>Service Link</t>
   </si>
   <si>
-    <t>IdServicio</t>
+    <t>92d914e8-9529-443d-9068-ed8a1d60cf6d</t>
+  </si>
+  <si>
+    <t>f801c129-5699-4ced-acf5-0aa1a7b07d4a</t>
+  </si>
+  <si>
+    <t>a8b2f011-29d9-42e0-b389-900fcbd04666</t>
+  </si>
+  <si>
+    <t>641e41a8-8069-4cb3-83e7-ec8306ae27c6</t>
+  </si>
+  <si>
+    <t>Servicios de Ingeniería.</t>
+  </si>
+  <si>
+    <t>Control de Procesos.</t>
+  </si>
+  <si>
+    <t>Diseño y Fabricación de Tableros</t>
+  </si>
+  <si>
+    <t>Integración de Redes Industriales</t>
   </si>
   <si>
     <t>/servicio1.jpg</t>
@@ -70,79 +97,19 @@
     <t>Desarrollamos plataformas robustas, seguras y escalables para tu empresa.</t>
   </si>
   <si>
-    <t>Diseño y desarrollo a medida de plataformas adaptadas a tus procesos.</t>
-  </si>
-  <si>
-    <t>Desarrollo de backend sólido y APIs seguras.</t>
-  </si>
-  <si>
-    <t>Refactorización de código y mejoras incrementales.</t>
-  </si>
-  <si>
-    <t>Soporte técnico con SLA y monitoreo activo.</t>
-  </si>
-  <si>
-    <t>Desarrollo específico para cada industria.</t>
-  </si>
-  <si>
-    <t>Diseñados para crecer con tu negocio.</t>
-  </si>
-  <si>
-    <t>Administra tus productos con facilidad.</t>
-  </si>
-  <si>
-    <t>Pagos seguros y rápidos.</t>
-  </si>
-  <si>
-    <t>Interfaces visuales modernas y fáciles de usar.; Sistemas internos seguros y eficientes para manejar datos.; Conexión con otras plataformas o sistemas que ya usas.; Control total de usuarios, permisos y accesos.; Paneles de administración intuitivos.</t>
-  </si>
-  <si>
-    <t>Desarrollo de APIs REST con C#, Python y Node.js.; Integración con bases de datos SQL Server, MySQL, MongoDB y Oracle.; Autenticación segura con JWT y OAuth 2.0.; Documentación de endpoints con Swagger / OpenAPI.; Uso de Blazor y React como frontends conectados a APIs robustas.</t>
-  </si>
-  <si>
-    <t>92d914e8-9529-443d-9068-ed8a1d60cf6d</t>
-  </si>
-  <si>
-    <t>f801c129-5699-4ced-acf5-0aa1a7b07d4a</t>
-  </si>
-  <si>
-    <t>a8b2f011-29d9-42e0-b389-900fcbd04666</t>
-  </si>
-  <si>
-    <t>641e41a8-8069-4cb3-83e7-ec8306ae27c6</t>
-  </si>
-  <si>
-    <t>Orden</t>
-  </si>
-  <si>
-    <t>Actualización de librerías.; Optimización de rendimiento.; Revisión técnica periódica.; Mejoras visuales y funcionales basadas en feedback de usuarios.; Adaptación a nuevas tendencias tecnológicas y estándares de desarrollo.</t>
-  </si>
-  <si>
-    <t>Levantamiento y análisis de necesidades reales del negocio.; Diseño de arquitectura tecnológica adaptada al proyecto.; Automatización de procesos internos para mayor eficiencia.; Integración con sistemas existentes (ERP, CRM, etc.).</t>
-  </si>
-  <si>
-    <t>Carga masiva de productos desde archivos Excel o CSV.; Control automático de stock, precios y disponibilidad.; Descripciones optimizadas para buscadores (SEO).; Clasificación por categorías, filtros y etiquetas personalizadas.</t>
-  </si>
-  <si>
-    <t>Webpay, PayPal, MercadoPago, OneClick.; Boletas electrónicas automáticas.; Facturas electrónicas.; Envíos e integración logística.</t>
-  </si>
-  <si>
-    <t>Estructura modular que permite agregar nuevas funciones fácilmente.; Soporte para trabajar en distintos ambientes (desarrollo, pruebas y producción).; Automatización de despliegues para actualizaciones rápidas y seguras.; Preparado para manejar mayor cantidad de usuarios o datos sin perder rendimiento.</t>
-  </si>
-  <si>
-    <t>Resolución rápida de errores técnicos.; Prevención proactiva de incidentes.; Monitoreo con Grafana, Sentry o Prometheus.; Informes de estabilidad y rendimiento.; Soporte con SLA y canales directos.</t>
-  </si>
-  <si>
-    <t>Servicios de Ingeniería.</t>
-  </si>
-  <si>
-    <t>Control de Procesos.</t>
-  </si>
-  <si>
-    <t>Servicios Especializados.</t>
-  </si>
-  <si>
-    <t>Especialidad Eléctrica y Eléctricos</t>
+    <t>Optimización y eficiencia de procesos industriales.</t>
+  </si>
+  <si>
+    <t>Fabricamos tableros eléctricos para control y fuerza, diseñados según normas vigentes para faenas y plantas industriales.</t>
+  </si>
+  <si>
+    <t>Implementamos sistemas SCADA y HMI para supervisión remota, trazabilidad y eficiencia operativa en tiempo real.</t>
+  </si>
+  <si>
+    <t>Integramos redes industriales seguras y robustas, compatibles con múltiples protocolos: Profinet, Modbus, OPC-UA.</t>
+  </si>
+  <si>
+    <t>Dictamos cursos en programación de PLCs, redes industriales, SCADA, IoT y normativas eléctricas para profesionales.</t>
   </si>
   <si>
     <t>linear-gradient(180deg, #4a1f1f, #702d2d)</t>
@@ -157,27 +124,18 @@
     <t>linear-gradient(180deg, #4a441f, #70672d)</t>
   </si>
   <si>
+    <t>PrecisionManufacturingIcon</t>
+  </si>
+  <si>
+    <t>ShowChartIcon</t>
+  </si>
+  <si>
+    <t>BuildIcon</t>
+  </si>
+  <si>
     <t>ElectricalServicesIcon</t>
   </si>
   <si>
-    <t>BuildIcon</t>
-  </si>
-  <si>
-    <t>ShowChartIcon</t>
-  </si>
-  <si>
-    <t>PrecisionManufacturingIcon</t>
-  </si>
-  <si>
-    <t>Optimización y eficiencia de procesos industriales.</t>
-  </si>
-  <si>
-    <t>Soluciones a medida en ingeniería especializada.</t>
-  </si>
-  <si>
-    <t>Instalaciones eléctricas seguras y normadas.</t>
-  </si>
-  <si>
     <t>ÁREA ELÉCTRICA</t>
   </si>
   <si>
@@ -190,16 +148,40 @@
     <t>PROGRAMACIÓN SISTEMA DE CONTROL</t>
   </si>
   <si>
-    <t>GESTIÓN DE PROYECTOS</t>
-  </si>
-  <si>
-    <t>EVALUACIÓN DE PROYECTOS</t>
-  </si>
-  <si>
-    <t>ESPECIALIDAD ELÉCTRICA</t>
-  </si>
-  <si>
-    <t>ELÉCTRICOS</t>
+    <t>Tableros Eléctricos</t>
+  </si>
+  <si>
+    <t>SCADA y Supervisión</t>
+  </si>
+  <si>
+    <t>Redes y Protocolos</t>
+  </si>
+  <si>
+    <t>Formación Técnica</t>
+  </si>
+  <si>
+    <t>Ingeniería eléctrica aplicada a entornos industriales, desde el diseño hasta la ejecución en planta.</t>
+  </si>
+  <si>
+    <t>Diseño y revisión de arquitecturas de automatización y control, con foco en eficiencia y seguridad.</t>
+  </si>
+  <si>
+    <t>Desarrollo de sistemas de control industrial con PLCs y lógica de procesos personalizados.</t>
+  </si>
+  <si>
+    <t>Soporte técnico especializado en automatización, con monitoreo, diagnóstico y mejora continua.</t>
+  </si>
+  <si>
+    <t>Tableros de control y potencia diseñados a medida, cumpliendo con estándares de seguridad y funcionalidad industrial.</t>
+  </si>
+  <si>
+    <t>Sistemas de monitoreo y control para procesos industriales críticos, accesibles desde planta o vía remota.</t>
+  </si>
+  <si>
+    <t>Infraestructura de comunicación industrial confiable, ideal para entornos exigentes y sistemas distribuidos.</t>
+  </si>
+  <si>
+    <t>Programas de capacitación técnica diseñados por ingenieros expertos con experiencia en terreno y normativa actualizada.</t>
   </si>
   <si>
     <t>/area-electrica-1.jpg</t>
@@ -230,6 +212,30 @@
   <si>
     <t xml:space="preserve">/4-Electricos.jpg
 </t>
+  </si>
+  <si>
+    <t>Estudios eléctricos para planta y faena.;Diseño bajo normativas vigentes.;Cálculo y selección de componentes.;Supervisión técnica en terreno.</t>
+  </si>
+  <si>
+    <t>Levantamiento y documentación de procesos.;Diseño lógico de sistemas de control.;Validación funcional y revisión técnica.;Normativas eléctricas y de seguridad.</t>
+  </si>
+  <si>
+    <t>Programación de PLC Siemens, Rockwell, Schneider.;Lógica secuencial y control PID.;Simulación y pruebas funcionales.;Integración con HMI y SCADA.</t>
+  </si>
+  <si>
+    <t>Diagnóstico remoto de sistemas de control.;Soporte técnico post-implementación.;Actualización de software y firmware.;Mejora de eficiencia operativa.</t>
+  </si>
+  <si>
+    <t>Diseño de tableros de fuerza y control.;Fabricación con componentes certificados.;Montaje y pruebas en taller.;Entrega con planos y manuales técnicos.</t>
+  </si>
+  <si>
+    <t>Desarrollo SCADA con AVEVA, FactoryTalk, PCS7.;Integración con HMI y sensores.;Alarmas, reportes e historización.;Supervisión web en tiempo real.</t>
+  </si>
+  <si>
+    <t>Configuración de redes industriales.;Protocolos: Modbus, Profinet, OPC-UA.;Segmentación y ciberseguridad OT.;Diagnóstico y monitoreo de red.</t>
+  </si>
+  <si>
+    <t>Cursos de PLC Siemens, Delta, Schneider.;SCADA e integración con HMI.;Redes industriales: Profibus, OPC.;IoT industrial y normativas eléctricas.</t>
   </si>
 </sst>
 </file>
@@ -305,7 +311,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -613,342 +621,335 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="63.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
-    <col min="11" max="11" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="138" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>25</v>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>38</v>
+      <c r="C4" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>62</v>
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>38</v>
+      <c r="C5" t="s">
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>36</v>
+      <c r="J5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>39</v>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>32</v>
+      <c r="J6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>39</v>
+      <c r="C7" t="s">
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>35</v>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>40</v>
+      <c r="C8" t="s">
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>33</v>
+      <c r="I8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>34</v>
+      <c r="I9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -961,6 +962,5 @@
     <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>